<commit_message>
run_classifier works, corresponding changes to run_squad, added tensorboard_api
run_classifier:
- created SquadProcessor
- loads pickled results from run_squad
  - train-v2.0-pickled
  - dev-v2.0-pickled
- binary classification is_impossible
- writes results to txt file, and
- writes pickled dict predict_is_impossible[qid: 1]

run_squad
- changed naming convention of cached files to add True/False for
   --add_triviaqa_train
   --tiny_data
- added save_squad_examples to pickle dump the train and dev examples for run_classifier.py

tensorboard_api
- found this script to allow pytorch logging to tensorboard
</commit_message>
<xml_diff>
--- a/examples/output/190313-12_56-errors.xlsx
+++ b/examples/output/190313-12_56-errors.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klalande/Box Sync/klalande/Kevin/Online Courses/2017 Stanford Graduate Certificate/CS224/02_Project/01_Code/pytorch-pretrained-BERT/examples/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B7FE84-DA25-3E44-AD28-7AB59FAFC366}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25700" windowHeight="11480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="errorAnalysis" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -139,8 +152,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +216,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -249,7 +270,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,9 +302,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,6 +354,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,30 +547,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:AC466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="3:29">
+    <row r="3" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>72.65547877591312</v>
-      </c>
-    </row>
-    <row r="4" spans="3:29">
+        <v>72.655478775913124</v>
+      </c>
+    </row>
+    <row r="4" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>75.64352872538917</v>
-      </c>
-    </row>
-    <row r="5" spans="3:29">
+        <v>75.643528725389174</v>
+      </c>
+    </row>
+    <row r="5" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
@@ -521,7 +580,7 @@
         <v>6078</v>
       </c>
     </row>
-    <row r="6" spans="3:29">
+    <row r="6" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -529,15 +588,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:29">
+    <row r="7" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>79.40111878907535</v>
-      </c>
-    </row>
-    <row r="8" spans="3:29">
+        <v>79.401118789075355</v>
+      </c>
+    </row>
+    <row r="8" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
@@ -545,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:29">
+    <row r="9" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
@@ -553,7 +612,7 @@
         <v>6078</v>
       </c>
     </row>
-    <row r="11" spans="3:29">
+    <row r="11" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>15</v>
       </c>
@@ -567,7 +626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="3:29">
+    <row r="12" spans="3:29" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
@@ -617,7 +676,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="3:29">
+    <row r="13" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
@@ -679,7 +738,7 @@
         <v>2552</v>
       </c>
     </row>
-    <row r="14" spans="3:29">
+    <row r="14" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
@@ -741,7 +800,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="3:29">
+    <row r="15" spans="3:29" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f>SUM(D13:D14)</f>
+        <v>1349</v>
+      </c>
+      <c r="E15">
+        <f>SUM(E13:E14)</f>
+        <v>4416</v>
+      </c>
+      <c r="F15">
+        <f>SUM(F13:F14)</f>
+        <v>313</v>
+      </c>
+      <c r="G15">
+        <f>SUM(G13:G14)</f>
+        <v>6078</v>
+      </c>
       <c r="K15" s="1">
         <v>217</v>
       </c>
@@ -788,7 +863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="3:29">
+    <row r="16" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K16" s="1">
         <v>275</v>
       </c>
@@ -835,7 +910,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="3:29">
+    <row r="17" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>36</v>
       </c>
@@ -885,7 +960,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="18" spans="3:29">
+    <row r="18" spans="3:29" x14ac:dyDescent="0.2">
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
@@ -944,7 +1019,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="3:29">
+    <row r="19" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1006,7 +1081,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="3:29">
+    <row r="20" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
@@ -1068,7 +1143,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="3:29">
+    <row r="21" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1130,7 +1205,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="3:29">
+    <row r="22" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1192,7 +1267,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="3:29">
+    <row r="23" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1254,7 +1329,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="3:29">
+    <row r="24" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1316,7 +1391,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="3:29">
+    <row r="25" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1378,7 +1453,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="3:29">
+    <row r="26" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1440,7 +1515,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="3:29">
+    <row r="27" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1502,7 +1577,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="3:29">
+    <row r="28" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>25</v>
       </c>
@@ -1564,7 +1639,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="3:29">
+    <row r="29" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1626,7 +1701,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="3:29">
+    <row r="30" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1763,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="3:29">
+    <row r="31" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1750,7 +1825,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="3:29">
+    <row r="32" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1812,7 +1887,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="3:29">
+    <row r="33" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1874,7 +1949,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="3:29">
+    <row r="34" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1936,7 +2011,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="3:29">
+    <row r="35" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1998,7 +2073,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="3:29">
+    <row r="36" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C36" s="1" t="s">
         <v>33</v>
       </c>
@@ -2060,7 +2135,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="3:29">
+    <row r="37" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C37" s="1" t="s">
         <v>34</v>
       </c>
@@ -2122,7 +2197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="3:29">
+    <row r="38" spans="3:29" x14ac:dyDescent="0.2">
       <c r="C38" s="1" t="s">
         <v>35</v>
       </c>
@@ -2184,7 +2259,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="3:29">
+    <row r="39" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K39" s="1">
         <v>467</v>
       </c>
@@ -2231,7 +2306,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="3:29">
+    <row r="40" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K40" s="1">
         <v>469</v>
       </c>
@@ -2278,7 +2353,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="3:29">
+    <row r="41" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K41" s="1">
         <v>474</v>
       </c>
@@ -2325,7 +2400,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="3:29">
+    <row r="42" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K42" s="1">
         <v>478</v>
       </c>
@@ -2372,7 +2447,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="3:29">
+    <row r="43" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K43" s="1">
         <v>482</v>
       </c>
@@ -2419,7 +2494,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="3:29">
+    <row r="44" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K44" s="1">
         <v>499</v>
       </c>
@@ -2466,7 +2541,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="3:29">
+    <row r="45" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K45" s="1">
         <v>500</v>
       </c>
@@ -2513,7 +2588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="3:29">
+    <row r="46" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K46" s="1">
         <v>501</v>
       </c>
@@ -2560,7 +2635,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="3:29">
+    <row r="47" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K47" s="1">
         <v>502</v>
       </c>
@@ -2607,7 +2682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="3:29">
+    <row r="48" spans="3:29" x14ac:dyDescent="0.2">
       <c r="K48" s="1">
         <v>503</v>
       </c>
@@ -2654,7 +2729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="11:29">
+    <row r="49" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K49" s="1">
         <v>505</v>
       </c>
@@ -2701,7 +2776,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="11:29">
+    <row r="50" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K50" s="1">
         <v>507</v>
       </c>
@@ -2748,7 +2823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="11:29">
+    <row r="51" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K51" s="1">
         <v>508</v>
       </c>
@@ -2795,7 +2870,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="11:29">
+    <row r="52" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K52" s="1">
         <v>510</v>
       </c>
@@ -2842,7 +2917,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="11:29">
+    <row r="53" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K53" s="1">
         <v>511</v>
       </c>
@@ -2889,7 +2964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="11:29">
+    <row r="54" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K54" s="1">
         <v>513</v>
       </c>
@@ -2936,7 +3011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="11:29">
+    <row r="55" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K55" s="1">
         <v>514</v>
       </c>
@@ -2983,7 +3058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="11:29">
+    <row r="56" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K56" s="1">
         <v>516</v>
       </c>
@@ -3030,7 +3105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="11:29">
+    <row r="57" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K57" s="1">
         <v>518</v>
       </c>
@@ -3077,7 +3152,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="11:29">
+    <row r="58" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K58" s="1">
         <v>519</v>
       </c>
@@ -3124,7 +3199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="11:29">
+    <row r="59" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K59" s="1">
         <v>520</v>
       </c>
@@ -3171,7 +3246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="11:29">
+    <row r="60" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K60" s="1">
         <v>522</v>
       </c>
@@ -3218,7 +3293,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="11:29">
+    <row r="61" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K61" s="1">
         <v>523</v>
       </c>
@@ -3265,7 +3340,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="11:29">
+    <row r="62" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K62" s="1">
         <v>524</v>
       </c>
@@ -3312,7 +3387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="11:29">
+    <row r="63" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K63" s="1">
         <v>527</v>
       </c>
@@ -3359,7 +3434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="11:29">
+    <row r="64" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K64" s="1">
         <v>529</v>
       </c>
@@ -3406,7 +3481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="11:29">
+    <row r="65" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K65" s="1">
         <v>531</v>
       </c>
@@ -3453,7 +3528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="11:29">
+    <row r="66" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K66" s="1">
         <v>532</v>
       </c>
@@ -3500,7 +3575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="11:29">
+    <row r="67" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K67" s="1">
         <v>534</v>
       </c>
@@ -3547,7 +3622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="11:29">
+    <row r="68" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K68" s="1">
         <v>535</v>
       </c>
@@ -3594,7 +3669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="11:29">
+    <row r="69" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K69" s="1">
         <v>536</v>
       </c>
@@ -3641,7 +3716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="11:29">
+    <row r="70" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K70" s="1">
         <v>538</v>
       </c>
@@ -3688,7 +3763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="11:29">
+    <row r="71" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K71" s="1">
         <v>539</v>
       </c>
@@ -3735,7 +3810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="11:29">
+    <row r="72" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K72" s="1">
         <v>541</v>
       </c>
@@ -3782,7 +3857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="11:29">
+    <row r="73" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K73" s="1">
         <v>542</v>
       </c>
@@ -3829,7 +3904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="11:29">
+    <row r="74" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K74" s="1">
         <v>543</v>
       </c>
@@ -3876,7 +3951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="11:29">
+    <row r="75" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K75" s="1">
         <v>544</v>
       </c>
@@ -3923,7 +3998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="11:29">
+    <row r="76" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K76" s="1">
         <v>545</v>
       </c>
@@ -3970,7 +4045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="11:29">
+    <row r="77" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K77" s="1">
         <v>546</v>
       </c>
@@ -4017,7 +4092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="11:29">
+    <row r="78" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K78" s="1">
         <v>548</v>
       </c>
@@ -4064,7 +4139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="11:29">
+    <row r="79" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K79" s="1">
         <v>549</v>
       </c>
@@ -4111,7 +4186,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="11:29">
+    <row r="80" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K80" s="1">
         <v>550</v>
       </c>
@@ -4158,7 +4233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="11:29">
+    <row r="81" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K81" s="1">
         <v>551</v>
       </c>
@@ -4205,7 +4280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="11:29">
+    <row r="82" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K82" s="1">
         <v>552</v>
       </c>
@@ -4252,7 +4327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="11:29">
+    <row r="83" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K83" s="1">
         <v>553</v>
       </c>
@@ -4299,7 +4374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="11:29">
+    <row r="84" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K84" s="1">
         <v>554</v>
       </c>
@@ -4346,7 +4421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="11:29">
+    <row r="85" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K85" s="1">
         <v>555</v>
       </c>
@@ -4393,7 +4468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="11:29">
+    <row r="86" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K86" s="1">
         <v>556</v>
       </c>
@@ -4440,7 +4515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="11:29">
+    <row r="87" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K87" s="1">
         <v>557</v>
       </c>
@@ -4487,7 +4562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="11:29">
+    <row r="88" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K88" s="1">
         <v>559</v>
       </c>
@@ -4534,7 +4609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="11:29">
+    <row r="89" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K89" s="1">
         <v>561</v>
       </c>
@@ -4581,7 +4656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="11:29">
+    <row r="90" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K90" s="1">
         <v>562</v>
       </c>
@@ -4628,7 +4703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="11:29">
+    <row r="91" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K91" s="1">
         <v>564</v>
       </c>
@@ -4675,7 +4750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="11:29">
+    <row r="92" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K92" s="1">
         <v>565</v>
       </c>
@@ -4722,7 +4797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="11:29">
+    <row r="93" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K93" s="1">
         <v>566</v>
       </c>
@@ -4769,7 +4844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="11:29">
+    <row r="94" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K94" s="1">
         <v>567</v>
       </c>
@@ -4816,7 +4891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="11:29">
+    <row r="95" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K95" s="1">
         <v>568</v>
       </c>
@@ -4863,7 +4938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="11:29">
+    <row r="96" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K96" s="1">
         <v>569</v>
       </c>
@@ -4910,7 +4985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="11:29">
+    <row r="97" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K97" s="1">
         <v>571</v>
       </c>
@@ -4957,7 +5032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="11:29">
+    <row r="98" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K98" s="1">
         <v>575</v>
       </c>
@@ -5004,7 +5079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="11:29">
+    <row r="99" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K99" s="1">
         <v>576</v>
       </c>
@@ -5051,7 +5126,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="11:29">
+    <row r="100" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K100" s="1">
         <v>577</v>
       </c>
@@ -5098,7 +5173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="11:29">
+    <row r="101" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K101" s="1">
         <v>578</v>
       </c>
@@ -5145,7 +5220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="11:29">
+    <row r="102" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K102" s="1">
         <v>580</v>
       </c>
@@ -5192,7 +5267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="11:29">
+    <row r="103" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K103" s="1">
         <v>581</v>
       </c>
@@ -5239,7 +5314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="11:29">
+    <row r="104" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K104" s="1">
         <v>582</v>
       </c>
@@ -5286,7 +5361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="11:29">
+    <row r="105" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K105" s="1">
         <v>584</v>
       </c>
@@ -5333,7 +5408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="11:29">
+    <row r="106" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K106" s="1">
         <v>585</v>
       </c>
@@ -5380,7 +5455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="11:29">
+    <row r="107" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K107" s="1">
         <v>587</v>
       </c>
@@ -5427,7 +5502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="11:29">
+    <row r="108" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K108" s="1">
         <v>588</v>
       </c>
@@ -5474,7 +5549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="11:29">
+    <row r="109" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K109" s="1">
         <v>590</v>
       </c>
@@ -5521,7 +5596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="11:29">
+    <row r="110" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K110" s="1">
         <v>591</v>
       </c>
@@ -5568,7 +5643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="11:29">
+    <row r="111" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K111" s="1">
         <v>592</v>
       </c>
@@ -5615,7 +5690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="11:29">
+    <row r="112" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K112" s="1">
         <v>594</v>
       </c>
@@ -5662,7 +5737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="11:29">
+    <row r="113" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K113" s="1">
         <v>597</v>
       </c>
@@ -5709,7 +5784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="11:29">
+    <row r="114" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K114" s="1">
         <v>598</v>
       </c>
@@ -5756,7 +5831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="11:29">
+    <row r="115" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K115" s="1">
         <v>599</v>
       </c>
@@ -5803,7 +5878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="11:29">
+    <row r="116" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K116" s="1">
         <v>600</v>
       </c>
@@ -5850,7 +5925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="11:29">
+    <row r="117" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K117" s="1">
         <v>601</v>
       </c>
@@ -5897,7 +5972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="11:29">
+    <row r="118" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K118" s="1">
         <v>602</v>
       </c>
@@ -5944,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="11:29">
+    <row r="119" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K119" s="1">
         <v>603</v>
       </c>
@@ -5991,7 +6066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="11:29">
+    <row r="120" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K120" s="1">
         <v>604</v>
       </c>
@@ -6038,7 +6113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="11:29">
+    <row r="121" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K121" s="1">
         <v>605</v>
       </c>
@@ -6085,7 +6160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="11:29">
+    <row r="122" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K122" s="1">
         <v>606</v>
       </c>
@@ -6132,7 +6207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="11:29">
+    <row r="123" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K123" s="1">
         <v>608</v>
       </c>
@@ -6179,7 +6254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="11:29">
+    <row r="124" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K124" s="1">
         <v>609</v>
       </c>
@@ -6226,7 +6301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="11:29">
+    <row r="125" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K125" s="1">
         <v>610</v>
       </c>
@@ -6273,7 +6348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="11:29">
+    <row r="126" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K126" s="1">
         <v>611</v>
       </c>
@@ -6320,7 +6395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="11:29">
+    <row r="127" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K127" s="1">
         <v>612</v>
       </c>
@@ -6367,7 +6442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="11:29">
+    <row r="128" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K128" s="1">
         <v>613</v>
       </c>
@@ -6414,7 +6489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="11:29">
+    <row r="129" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K129" s="1">
         <v>614</v>
       </c>
@@ -6461,7 +6536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="11:29">
+    <row r="130" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K130" s="1">
         <v>615</v>
       </c>
@@ -6508,7 +6583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="11:29">
+    <row r="131" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K131" s="1">
         <v>616</v>
       </c>
@@ -6555,7 +6630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="11:29">
+    <row r="132" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K132" s="1">
         <v>617</v>
       </c>
@@ -6602,7 +6677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="11:29">
+    <row r="133" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K133" s="1">
         <v>618</v>
       </c>
@@ -6649,7 +6724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="11:29">
+    <row r="134" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K134" s="1">
         <v>619</v>
       </c>
@@ -6696,7 +6771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="11:29">
+    <row r="135" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K135" s="1">
         <v>620</v>
       </c>
@@ -6743,7 +6818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="11:29">
+    <row r="136" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K136" s="1">
         <v>622</v>
       </c>
@@ -6790,7 +6865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="11:29">
+    <row r="137" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K137" s="1">
         <v>623</v>
       </c>
@@ -6837,7 +6912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="11:29">
+    <row r="138" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K138" s="1">
         <v>625</v>
       </c>
@@ -6884,7 +6959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="11:29">
+    <row r="139" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K139" s="1">
         <v>626</v>
       </c>
@@ -6931,7 +7006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="11:29">
+    <row r="140" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K140" s="1">
         <v>627</v>
       </c>
@@ -6978,7 +7053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="11:29">
+    <row r="141" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K141" s="1">
         <v>628</v>
       </c>
@@ -7025,7 +7100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="11:29">
+    <row r="142" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K142" s="1">
         <v>630</v>
       </c>
@@ -7072,7 +7147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="11:29">
+    <row r="143" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K143" s="1">
         <v>631</v>
       </c>
@@ -7119,7 +7194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="11:29">
+    <row r="144" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K144" s="1">
         <v>632</v>
       </c>
@@ -7166,7 +7241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="11:29">
+    <row r="145" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K145" s="1">
         <v>633</v>
       </c>
@@ -7213,7 +7288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="11:29">
+    <row r="146" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K146" s="1">
         <v>634</v>
       </c>
@@ -7245,7 +7320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="11:29">
+    <row r="147" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K147" s="1">
         <v>635</v>
       </c>
@@ -7277,7 +7352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="11:29">
+    <row r="148" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K148" s="1">
         <v>636</v>
       </c>
@@ -7309,7 +7384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="11:29">
+    <row r="149" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K149" s="1">
         <v>637</v>
       </c>
@@ -7341,7 +7416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="11:29">
+    <row r="150" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K150" s="1">
         <v>638</v>
       </c>
@@ -7373,7 +7448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="11:29">
+    <row r="151" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K151" s="1">
         <v>639</v>
       </c>
@@ -7405,7 +7480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="11:29">
+    <row r="152" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K152" s="1">
         <v>641</v>
       </c>
@@ -7437,7 +7512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="11:29">
+    <row r="153" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K153" s="1">
         <v>642</v>
       </c>
@@ -7469,7 +7544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="11:29">
+    <row r="154" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K154" s="1">
         <v>643</v>
       </c>
@@ -7501,7 +7576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="11:29">
+    <row r="155" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K155" s="1">
         <v>644</v>
       </c>
@@ -7533,7 +7608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="11:29">
+    <row r="156" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K156" s="1">
         <v>646</v>
       </c>
@@ -7565,7 +7640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="11:29">
+    <row r="157" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K157" s="1">
         <v>647</v>
       </c>
@@ -7582,7 +7657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="11:29">
+    <row r="158" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K158" s="1">
         <v>648</v>
       </c>
@@ -7599,7 +7674,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="159" spans="11:29">
+    <row r="159" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K159" s="1">
         <v>650</v>
       </c>
@@ -7616,7 +7691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="11:29">
+    <row r="160" spans="11:29" x14ac:dyDescent="0.2">
       <c r="K160" s="1">
         <v>651</v>
       </c>
@@ -7633,7 +7708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="11:15">
+    <row r="161" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K161" s="1">
         <v>652</v>
       </c>
@@ -7650,7 +7725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="11:15">
+    <row r="162" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K162" s="1">
         <v>658</v>
       </c>
@@ -7667,7 +7742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="11:15">
+    <row r="163" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K163" s="1">
         <v>659</v>
       </c>
@@ -7684,7 +7759,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="11:15">
+    <row r="164" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K164" s="1">
         <v>662</v>
       </c>
@@ -7701,7 +7776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="11:15">
+    <row r="165" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K165" s="1">
         <v>663</v>
       </c>
@@ -7718,7 +7793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="11:15">
+    <row r="166" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K166" s="1">
         <v>665</v>
       </c>
@@ -7735,7 +7810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="11:15">
+    <row r="167" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K167" s="1">
         <v>666</v>
       </c>
@@ -7752,7 +7827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="11:15">
+    <row r="168" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K168" s="1">
         <v>667</v>
       </c>
@@ -7769,7 +7844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="11:15">
+    <row r="169" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K169" s="1">
         <v>668</v>
       </c>
@@ -7786,7 +7861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="11:15">
+    <row r="170" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K170" s="1">
         <v>669</v>
       </c>
@@ -7803,7 +7878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="11:15">
+    <row r="171" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K171" s="1">
         <v>671</v>
       </c>
@@ -7820,7 +7895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="172" spans="11:15">
+    <row r="172" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K172" s="1">
         <v>673</v>
       </c>
@@ -7837,7 +7912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="11:15">
+    <row r="173" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K173" s="1">
         <v>674</v>
       </c>
@@ -7854,7 +7929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="11:15">
+    <row r="174" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K174" s="1">
         <v>675</v>
       </c>
@@ -7871,7 +7946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="11:15">
+    <row r="175" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K175" s="1">
         <v>676</v>
       </c>
@@ -7888,7 +7963,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="176" spans="11:15">
+    <row r="176" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K176" s="1">
         <v>677</v>
       </c>
@@ -7905,7 +7980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="11:15">
+    <row r="177" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K177" s="1">
         <v>680</v>
       </c>
@@ -7922,7 +7997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="11:15">
+    <row r="178" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K178" s="1">
         <v>682</v>
       </c>
@@ -7939,7 +8014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="11:15">
+    <row r="179" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K179" s="1">
         <v>683</v>
       </c>
@@ -7956,7 +8031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="11:15">
+    <row r="180" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K180" s="1">
         <v>685</v>
       </c>
@@ -7973,7 +8048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="11:15">
+    <row r="181" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K181" s="1">
         <v>686</v>
       </c>
@@ -7990,7 +8065,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="11:15">
+    <row r="182" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K182" s="1">
         <v>687</v>
       </c>
@@ -8007,7 +8082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="11:15">
+    <row r="183" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K183" s="1">
         <v>688</v>
       </c>
@@ -8024,7 +8099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="184" spans="11:15">
+    <row r="184" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K184" s="1">
         <v>689</v>
       </c>
@@ -8041,7 +8116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="11:15">
+    <row r="185" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K185" s="1">
         <v>692</v>
       </c>
@@ -8058,7 +8133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="11:15">
+    <row r="186" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K186" s="1">
         <v>693</v>
       </c>
@@ -8075,7 +8150,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="187" spans="11:15">
+    <row r="187" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K187" s="1">
         <v>696</v>
       </c>
@@ -8092,7 +8167,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="188" spans="11:15">
+    <row r="188" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K188" s="1">
         <v>697</v>
       </c>
@@ -8109,7 +8184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="11:15">
+    <row r="189" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K189" s="1">
         <v>698</v>
       </c>
@@ -8126,7 +8201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="11:15">
+    <row r="190" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K190" s="1">
         <v>699</v>
       </c>
@@ -8143,7 +8218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="11:15">
+    <row r="191" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K191" s="1">
         <v>700</v>
       </c>
@@ -8160,7 +8235,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="192" spans="11:15">
+    <row r="192" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K192" s="1">
         <v>701</v>
       </c>
@@ -8177,7 +8252,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="11:15">
+    <row r="193" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K193" s="1">
         <v>702</v>
       </c>
@@ -8194,7 +8269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="11:15">
+    <row r="194" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K194" s="1">
         <v>703</v>
       </c>
@@ -8211,7 +8286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="11:15">
+    <row r="195" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K195" s="1">
         <v>705</v>
       </c>
@@ -8228,7 +8303,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="196" spans="11:15">
+    <row r="196" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K196" s="1">
         <v>706</v>
       </c>
@@ -8245,7 +8320,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="11:15">
+    <row r="197" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K197" s="1">
         <v>708</v>
       </c>
@@ -8262,7 +8337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="11:15">
+    <row r="198" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K198" s="1">
         <v>709</v>
       </c>
@@ -8279,7 +8354,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="199" spans="11:15">
+    <row r="199" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K199" s="1">
         <v>711</v>
       </c>
@@ -8296,7 +8371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="11:15">
+    <row r="200" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K200" s="1">
         <v>713</v>
       </c>
@@ -8313,7 +8388,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="201" spans="11:15">
+    <row r="201" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K201" s="1">
         <v>714</v>
       </c>
@@ -8330,7 +8405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="11:15">
+    <row r="202" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K202" s="1">
         <v>715</v>
       </c>
@@ -8347,7 +8422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="203" spans="11:15">
+    <row r="203" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K203" s="1">
         <v>716</v>
       </c>
@@ -8364,7 +8439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="11:15">
+    <row r="204" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K204" s="1">
         <v>717</v>
       </c>
@@ -8381,7 +8456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="205" spans="11:15">
+    <row r="205" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K205" s="1">
         <v>718</v>
       </c>
@@ -8398,7 +8473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="11:15">
+    <row r="206" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K206" s="1">
         <v>721</v>
       </c>
@@ -8415,7 +8490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="11:15">
+    <row r="207" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K207" s="1">
         <v>722</v>
       </c>
@@ -8432,7 +8507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="11:15">
+    <row r="208" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K208" s="1">
         <v>724</v>
       </c>
@@ -8449,7 +8524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="11:15">
+    <row r="209" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K209" s="1">
         <v>725</v>
       </c>
@@ -8466,7 +8541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="11:15">
+    <row r="210" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K210" s="1">
         <v>727</v>
       </c>
@@ -8483,7 +8558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211" spans="11:15">
+    <row r="211" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K211" s="1">
         <v>728</v>
       </c>
@@ -8500,7 +8575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="11:15">
+    <row r="212" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K212" s="1">
         <v>731</v>
       </c>
@@ -8517,7 +8592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="11:15">
+    <row r="213" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K213" s="1">
         <v>733</v>
       </c>
@@ -8534,7 +8609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="11:15">
+    <row r="214" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K214" s="1">
         <v>734</v>
       </c>
@@ -8551,7 +8626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="11:15">
+    <row r="215" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K215" s="1">
         <v>738</v>
       </c>
@@ -8568,7 +8643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="11:15">
+    <row r="216" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K216" s="1">
         <v>739</v>
       </c>
@@ -8585,7 +8660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="11:15">
+    <row r="217" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K217" s="1">
         <v>742</v>
       </c>
@@ -8602,7 +8677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="218" spans="11:15">
+    <row r="218" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K218" s="1">
         <v>743</v>
       </c>
@@ -8619,7 +8694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="219" spans="11:15">
+    <row r="219" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K219" s="1">
         <v>749</v>
       </c>
@@ -8636,7 +8711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="11:15">
+    <row r="220" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K220" s="1">
         <v>754</v>
       </c>
@@ -8653,7 +8728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="221" spans="11:15">
+    <row r="221" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K221" s="1">
         <v>755</v>
       </c>
@@ -8670,7 +8745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="11:15">
+    <row r="222" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K222" s="1">
         <v>757</v>
       </c>
@@ -8687,7 +8762,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="11:15">
+    <row r="223" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K223" s="1">
         <v>758</v>
       </c>
@@ -8704,7 +8779,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="224" spans="11:15">
+    <row r="224" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K224" s="1">
         <v>760</v>
       </c>
@@ -8721,7 +8796,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="225" spans="11:15">
+    <row r="225" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K225" s="1">
         <v>761</v>
       </c>
@@ -8738,7 +8813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" spans="11:15">
+    <row r="226" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K226" s="1">
         <v>762</v>
       </c>
@@ -8755,7 +8830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="227" spans="11:15">
+    <row r="227" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K227" s="1">
         <v>763</v>
       </c>
@@ -8772,7 +8847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="11:15">
+    <row r="228" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K228" s="1">
         <v>765</v>
       </c>
@@ -8789,7 +8864,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="229" spans="11:15">
+    <row r="229" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K229" s="1">
         <v>766</v>
       </c>
@@ -8806,7 +8881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="11:15">
+    <row r="230" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K230" s="1">
         <v>767</v>
       </c>
@@ -8823,7 +8898,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="231" spans="11:15">
+    <row r="231" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K231" s="1">
         <v>771</v>
       </c>
@@ -8840,7 +8915,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="232" spans="11:15">
+    <row r="232" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K232" s="1">
         <v>772</v>
       </c>
@@ -8857,7 +8932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="11:15">
+    <row r="233" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K233" s="1">
         <v>775</v>
       </c>
@@ -8874,7 +8949,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="11:15">
+    <row r="234" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K234" s="1">
         <v>778</v>
       </c>
@@ -8891,7 +8966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="235" spans="11:15">
+    <row r="235" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K235" s="1">
         <v>780</v>
       </c>
@@ -8908,7 +8983,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="11:15">
+    <row r="236" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K236" s="1">
         <v>782</v>
       </c>
@@ -8925,7 +9000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="11:15">
+    <row r="237" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K237" s="1">
         <v>783</v>
       </c>
@@ -8942,7 +9017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="11:15">
+    <row r="238" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K238" s="1">
         <v>784</v>
       </c>
@@ -8959,7 +9034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239" spans="11:15">
+    <row r="239" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K239" s="1">
         <v>787</v>
       </c>
@@ -8976,7 +9051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="11:15">
+    <row r="240" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K240" s="1">
         <v>790</v>
       </c>
@@ -8993,7 +9068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="11:15">
+    <row r="241" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K241" s="1">
         <v>793</v>
       </c>
@@ -9010,7 +9085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="242" spans="11:15">
+    <row r="242" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K242" s="1">
         <v>794</v>
       </c>
@@ -9027,7 +9102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="11:15">
+    <row r="243" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K243" s="1">
         <v>795</v>
       </c>
@@ -9044,7 +9119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244" spans="11:15">
+    <row r="244" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K244" s="1">
         <v>797</v>
       </c>
@@ -9061,7 +9136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="11:15">
+    <row r="245" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K245" s="1">
         <v>798</v>
       </c>
@@ -9078,7 +9153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="11:15">
+    <row r="246" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K246" s="1">
         <v>799</v>
       </c>
@@ -9095,7 +9170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="11:15">
+    <row r="247" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K247" s="1">
         <v>800</v>
       </c>
@@ -9112,7 +9187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248" spans="11:15">
+    <row r="248" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K248" s="1">
         <v>803</v>
       </c>
@@ -9129,7 +9204,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="249" spans="11:15">
+    <row r="249" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K249" s="1">
         <v>804</v>
       </c>
@@ -9146,7 +9221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="11:15">
+    <row r="250" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K250" s="1">
         <v>805</v>
       </c>
@@ -9163,7 +9238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="11:15">
+    <row r="251" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K251" s="1">
         <v>807</v>
       </c>
@@ -9180,7 +9255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="11:15">
+    <row r="252" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K252" s="1">
         <v>809</v>
       </c>
@@ -9197,7 +9272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="11:15">
+    <row r="253" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K253" s="1">
         <v>811</v>
       </c>
@@ -9214,7 +9289,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="254" spans="11:15">
+    <row r="254" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K254" s="1">
         <v>813</v>
       </c>
@@ -9231,7 +9306,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="255" spans="11:15">
+    <row r="255" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K255" s="1">
         <v>814</v>
       </c>
@@ -9248,7 +9323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="11:15">
+    <row r="256" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K256" s="1">
         <v>815</v>
       </c>
@@ -9265,7 +9340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="257" spans="11:15">
+    <row r="257" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K257" s="1">
         <v>818</v>
       </c>
@@ -9282,7 +9357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="11:15">
+    <row r="258" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K258" s="1">
         <v>819</v>
       </c>
@@ -9299,7 +9374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259" spans="11:15">
+    <row r="259" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K259" s="1">
         <v>820</v>
       </c>
@@ -9316,7 +9391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="11:15">
+    <row r="260" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K260" s="1">
         <v>821</v>
       </c>
@@ -9333,7 +9408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="11:15">
+    <row r="261" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K261" s="1">
         <v>824</v>
       </c>
@@ -9350,7 +9425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="11:15">
+    <row r="262" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K262" s="1">
         <v>825</v>
       </c>
@@ -9367,7 +9442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="11:15">
+    <row r="263" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K263" s="1">
         <v>826</v>
       </c>
@@ -9384,7 +9459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="264" spans="11:15">
+    <row r="264" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K264" s="1">
         <v>829</v>
       </c>
@@ -9401,7 +9476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="11:15">
+    <row r="265" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K265" s="1">
         <v>831</v>
       </c>
@@ -9418,7 +9493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="11:15">
+    <row r="266" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K266" s="1">
         <v>832</v>
       </c>
@@ -9435,7 +9510,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="267" spans="11:15">
+    <row r="267" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K267" s="1">
         <v>835</v>
       </c>
@@ -9452,7 +9527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="268" spans="11:15">
+    <row r="268" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K268" s="1">
         <v>836</v>
       </c>
@@ -9469,7 +9544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="269" spans="11:15">
+    <row r="269" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K269" s="1">
         <v>837</v>
       </c>
@@ -9486,7 +9561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="11:15">
+    <row r="270" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K270" s="1">
         <v>838</v>
       </c>
@@ -9503,7 +9578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="271" spans="11:15">
+    <row r="271" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K271" s="1">
         <v>840</v>
       </c>
@@ -9520,7 +9595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="11:15">
+    <row r="272" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K272" s="1">
         <v>841</v>
       </c>
@@ -9537,7 +9612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="273" spans="11:15">
+    <row r="273" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K273" s="1">
         <v>842</v>
       </c>
@@ -9554,7 +9629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="11:15">
+    <row r="274" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K274" s="1">
         <v>846</v>
       </c>
@@ -9571,7 +9646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="11:15">
+    <row r="275" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K275" s="1">
         <v>854</v>
       </c>
@@ -9588,7 +9663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="11:15">
+    <row r="276" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K276" s="1">
         <v>855</v>
       </c>
@@ -9605,7 +9680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="11:15">
+    <row r="277" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K277" s="1">
         <v>856</v>
       </c>
@@ -9622,7 +9697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="11:15">
+    <row r="278" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K278" s="1">
         <v>861</v>
       </c>
@@ -9639,7 +9714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="11:15">
+    <row r="279" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K279" s="1">
         <v>865</v>
       </c>
@@ -9656,7 +9731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="11:15">
+    <row r="280" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K280" s="1">
         <v>866</v>
       </c>
@@ -9673,7 +9748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="281" spans="11:15">
+    <row r="281" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K281" s="1">
         <v>867</v>
       </c>
@@ -9690,7 +9765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="11:15">
+    <row r="282" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K282" s="1">
         <v>869</v>
       </c>
@@ -9707,7 +9782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="283" spans="11:15">
+    <row r="283" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K283" s="1">
         <v>870</v>
       </c>
@@ -9724,7 +9799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="11:15">
+    <row r="284" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K284" s="1">
         <v>871</v>
       </c>
@@ -9741,7 +9816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="285" spans="11:15">
+    <row r="285" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K285" s="1">
         <v>874</v>
       </c>
@@ -9758,7 +9833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="286" spans="11:15">
+    <row r="286" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K286" s="1">
         <v>876</v>
       </c>
@@ -9775,7 +9850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="11:15">
+    <row r="287" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K287" s="1">
         <v>878</v>
       </c>
@@ -9792,7 +9867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="288" spans="11:15">
+    <row r="288" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K288" s="1">
         <v>880</v>
       </c>
@@ -9809,7 +9884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289" spans="11:15">
+    <row r="289" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K289" s="1">
         <v>881</v>
       </c>
@@ -9826,7 +9901,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="290" spans="11:15">
+    <row r="290" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K290" s="1">
         <v>883</v>
       </c>
@@ -9843,7 +9918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="291" spans="11:15">
+    <row r="291" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K291" s="1">
         <v>884</v>
       </c>
@@ -9860,7 +9935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="292" spans="11:15">
+    <row r="292" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K292" s="1">
         <v>885</v>
       </c>
@@ -9877,7 +9952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="293" spans="11:15">
+    <row r="293" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K293" s="1">
         <v>896</v>
       </c>
@@ -9894,7 +9969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294" spans="11:15">
+    <row r="294" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K294" s="1">
         <v>900</v>
       </c>
@@ -9911,7 +9986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="295" spans="11:15">
+    <row r="295" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K295" s="1">
         <v>905</v>
       </c>
@@ -9928,7 +10003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="296" spans="11:15">
+    <row r="296" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K296" s="1">
         <v>906</v>
       </c>
@@ -9945,7 +10020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="297" spans="11:15">
+    <row r="297" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K297" s="1">
         <v>915</v>
       </c>
@@ -9962,7 +10037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="298" spans="11:15">
+    <row r="298" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K298" s="1">
         <v>916</v>
       </c>
@@ -9979,7 +10054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="299" spans="11:15">
+    <row r="299" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K299" s="1">
         <v>917</v>
       </c>
@@ -9996,7 +10071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="11:15">
+    <row r="300" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K300" s="1">
         <v>918</v>
       </c>
@@ -10013,7 +10088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="11:15">
+    <row r="301" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K301" s="1">
         <v>920</v>
       </c>
@@ -10030,7 +10105,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="302" spans="11:15">
+    <row r="302" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K302" s="1">
         <v>921</v>
       </c>
@@ -10047,7 +10122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="303" spans="11:15">
+    <row r="303" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K303" s="1">
         <v>924</v>
       </c>
@@ -10064,7 +10139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="11:15">
+    <row r="304" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K304" s="1">
         <v>925</v>
       </c>
@@ -10081,7 +10156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="305" spans="11:15">
+    <row r="305" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K305" s="1">
         <v>927</v>
       </c>
@@ -10098,7 +10173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="11:15">
+    <row r="306" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K306" s="1">
         <v>931</v>
       </c>
@@ -10115,7 +10190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="307" spans="11:15">
+    <row r="307" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K307" s="1">
         <v>933</v>
       </c>
@@ -10132,7 +10207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="308" spans="11:15">
+    <row r="308" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K308" s="1">
         <v>939</v>
       </c>
@@ -10149,7 +10224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="309" spans="11:15">
+    <row r="309" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K309" s="1">
         <v>940</v>
       </c>
@@ -10166,7 +10241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310" spans="11:15">
+    <row r="310" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K310" s="1">
         <v>941</v>
       </c>
@@ -10183,7 +10258,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="11:15">
+    <row r="311" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K311" s="1">
         <v>945</v>
       </c>
@@ -10200,7 +10275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="312" spans="11:15">
+    <row r="312" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K312" s="1">
         <v>947</v>
       </c>
@@ -10217,7 +10292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="313" spans="11:15">
+    <row r="313" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K313" s="1">
         <v>949</v>
       </c>
@@ -10234,7 +10309,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="314" spans="11:15">
+    <row r="314" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K314" s="1">
         <v>952</v>
       </c>
@@ -10251,7 +10326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="315" spans="11:15">
+    <row r="315" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K315" s="1">
         <v>954</v>
       </c>
@@ -10268,7 +10343,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="316" spans="11:15">
+    <row r="316" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K316" s="1">
         <v>956</v>
       </c>
@@ -10285,7 +10360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="317" spans="11:15">
+    <row r="317" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K317" s="1">
         <v>959</v>
       </c>
@@ -10302,7 +10377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="318" spans="11:15">
+    <row r="318" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K318" s="1">
         <v>961</v>
       </c>
@@ -10319,7 +10394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="319" spans="11:15">
+    <row r="319" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K319" s="1">
         <v>962</v>
       </c>
@@ -10336,7 +10411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="320" spans="11:15">
+    <row r="320" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K320" s="1">
         <v>966</v>
       </c>
@@ -10353,7 +10428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="321" spans="11:15">
+    <row r="321" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K321" s="1">
         <v>970</v>
       </c>
@@ -10370,7 +10445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322" spans="11:15">
+    <row r="322" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K322" s="1">
         <v>973</v>
       </c>
@@ -10387,7 +10462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="323" spans="11:15">
+    <row r="323" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K323" s="1">
         <v>975</v>
       </c>
@@ -10404,7 +10479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="324" spans="11:15">
+    <row r="324" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K324" s="1">
         <v>977</v>
       </c>
@@ -10421,7 +10496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="325" spans="11:15">
+    <row r="325" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K325" s="1">
         <v>982</v>
       </c>
@@ -10438,7 +10513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="326" spans="11:15">
+    <row r="326" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K326" s="1">
         <v>984</v>
       </c>
@@ -10455,7 +10530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327" spans="11:15">
+    <row r="327" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K327" s="1">
         <v>986</v>
       </c>
@@ -10472,7 +10547,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="328" spans="11:15">
+    <row r="328" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K328" s="1">
         <v>987</v>
       </c>
@@ -10489,7 +10564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="329" spans="11:15">
+    <row r="329" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K329" s="1">
         <v>989</v>
       </c>
@@ -10506,7 +10581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="330" spans="11:15">
+    <row r="330" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K330" s="1">
         <v>992</v>
       </c>
@@ -10523,7 +10598,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="331" spans="11:15">
+    <row r="331" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K331" s="1">
         <v>995</v>
       </c>
@@ -10540,7 +10615,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="332" spans="11:15">
+    <row r="332" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K332" s="1">
         <v>996</v>
       </c>
@@ -10557,7 +10632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="333" spans="11:15">
+    <row r="333" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K333" s="1">
         <v>997</v>
       </c>
@@ -10574,7 +10649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="334" spans="11:15">
+    <row r="334" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K334" s="1">
         <v>1004</v>
       </c>
@@ -10591,7 +10666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="335" spans="11:15">
+    <row r="335" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K335" s="1">
         <v>1008</v>
       </c>
@@ -10608,7 +10683,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="336" spans="11:15">
+    <row r="336" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K336" s="1">
         <v>1016</v>
       </c>
@@ -10625,7 +10700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="337" spans="11:15">
+    <row r="337" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K337" s="1">
         <v>1017</v>
       </c>
@@ -10642,7 +10717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="338" spans="11:15">
+    <row r="338" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K338" s="1">
         <v>1018</v>
       </c>
@@ -10659,7 +10734,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="339" spans="11:15">
+    <row r="339" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K339" s="1">
         <v>1020</v>
       </c>
@@ -10676,7 +10751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="340" spans="11:15">
+    <row r="340" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K340" s="1">
         <v>1023</v>
       </c>
@@ -10693,7 +10768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="11:15">
+    <row r="341" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K341" s="1">
         <v>1024</v>
       </c>
@@ -10710,7 +10785,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="342" spans="11:15">
+    <row r="342" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K342" s="1">
         <v>1025</v>
       </c>
@@ -10727,7 +10802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="343" spans="11:15">
+    <row r="343" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K343" s="1">
         <v>1028</v>
       </c>
@@ -10744,7 +10819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="344" spans="11:15">
+    <row r="344" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K344" s="1">
         <v>1031</v>
       </c>
@@ -10761,7 +10836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="345" spans="11:15">
+    <row r="345" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K345" s="1">
         <v>1032</v>
       </c>
@@ -10778,7 +10853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="346" spans="11:15">
+    <row r="346" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K346" s="1">
         <v>1034</v>
       </c>
@@ -10795,7 +10870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="347" spans="11:15">
+    <row r="347" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K347" s="1">
         <v>1039</v>
       </c>
@@ -10812,7 +10887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="348" spans="11:15">
+    <row r="348" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K348" s="1">
         <v>1041</v>
       </c>
@@ -10829,7 +10904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="349" spans="11:15">
+    <row r="349" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K349" s="1">
         <v>1043</v>
       </c>
@@ -10846,7 +10921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="350" spans="11:15">
+    <row r="350" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K350" s="1">
         <v>1044</v>
       </c>
@@ -10863,7 +10938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="351" spans="11:15">
+    <row r="351" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K351" s="1">
         <v>1049</v>
       </c>
@@ -10880,7 +10955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="352" spans="11:15">
+    <row r="352" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K352" s="1">
         <v>1051</v>
       </c>
@@ -10897,7 +10972,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="353" spans="11:15">
+    <row r="353" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K353" s="1">
         <v>1053</v>
       </c>
@@ -10914,7 +10989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="354" spans="11:15">
+    <row r="354" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K354" s="1">
         <v>1064</v>
       </c>
@@ -10931,7 +11006,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="355" spans="11:15">
+    <row r="355" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K355" s="1">
         <v>1073</v>
       </c>
@@ -10948,7 +11023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="356" spans="11:15">
+    <row r="356" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K356" s="1">
         <v>1076</v>
       </c>
@@ -10965,7 +11040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="357" spans="11:15">
+    <row r="357" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K357" s="1">
         <v>1077</v>
       </c>
@@ -10982,7 +11057,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="358" spans="11:15">
+    <row r="358" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K358" s="1">
         <v>1078</v>
       </c>
@@ -10999,7 +11074,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="359" spans="11:15">
+    <row r="359" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K359" s="1">
         <v>1081</v>
       </c>
@@ -11016,7 +11091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="360" spans="11:15">
+    <row r="360" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K360" s="1">
         <v>1082</v>
       </c>
@@ -11033,7 +11108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361" spans="11:15">
+    <row r="361" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K361" s="1">
         <v>1088</v>
       </c>
@@ -11050,7 +11125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="362" spans="11:15">
+    <row r="362" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K362" s="1">
         <v>1091</v>
       </c>
@@ -11067,7 +11142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="363" spans="11:15">
+    <row r="363" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K363" s="1">
         <v>1095</v>
       </c>
@@ -11084,7 +11159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="364" spans="11:15">
+    <row r="364" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K364" s="1">
         <v>1097</v>
       </c>
@@ -11101,7 +11176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="365" spans="11:15">
+    <row r="365" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K365" s="1">
         <v>1103</v>
       </c>
@@ -11118,7 +11193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="366" spans="11:15">
+    <row r="366" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K366" s="1">
         <v>1106</v>
       </c>
@@ -11135,7 +11210,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="367" spans="11:15">
+    <row r="367" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K367" s="1">
         <v>1107</v>
       </c>
@@ -11152,7 +11227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="368" spans="11:15">
+    <row r="368" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K368" s="1">
         <v>1112</v>
       </c>
@@ -11169,7 +11244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="369" spans="11:15">
+    <row r="369" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K369" s="1">
         <v>1113</v>
       </c>
@@ -11186,7 +11261,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="370" spans="11:15">
+    <row r="370" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K370" s="1">
         <v>1114</v>
       </c>
@@ -11203,7 +11278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="371" spans="11:15">
+    <row r="371" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K371" s="1">
         <v>1124</v>
       </c>
@@ -11220,7 +11295,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="372" spans="11:15">
+    <row r="372" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K372" s="1">
         <v>1135</v>
       </c>
@@ -11237,7 +11312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="373" spans="11:15">
+    <row r="373" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K373" s="1">
         <v>1137</v>
       </c>
@@ -11254,7 +11329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="374" spans="11:15">
+    <row r="374" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K374" s="1">
         <v>1138</v>
       </c>
@@ -11271,7 +11346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="375" spans="11:15">
+    <row r="375" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K375" s="1">
         <v>1140</v>
       </c>
@@ -11288,7 +11363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="376" spans="11:15">
+    <row r="376" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K376" s="1">
         <v>1146</v>
       </c>
@@ -11305,7 +11380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="377" spans="11:15">
+    <row r="377" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K377" s="1">
         <v>1150</v>
       </c>
@@ -11322,7 +11397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="378" spans="11:15">
+    <row r="378" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K378" s="1">
         <v>1151</v>
       </c>
@@ -11339,7 +11414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="379" spans="11:15">
+    <row r="379" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K379" s="1">
         <v>1152</v>
       </c>
@@ -11356,7 +11431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="380" spans="11:15">
+    <row r="380" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K380" s="1">
         <v>1153</v>
       </c>
@@ -11373,7 +11448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="11:15">
+    <row r="381" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K381" s="1">
         <v>1155</v>
       </c>
@@ -11390,7 +11465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="382" spans="11:15">
+    <row r="382" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K382" s="1">
         <v>1160</v>
       </c>
@@ -11407,7 +11482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="383" spans="11:15">
+    <row r="383" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K383" s="1">
         <v>1165</v>
       </c>
@@ -11424,7 +11499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="384" spans="11:15">
+    <row r="384" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K384" s="1">
         <v>1166</v>
       </c>
@@ -11441,7 +11516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="385" spans="11:15">
+    <row r="385" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K385" s="1">
         <v>1170</v>
       </c>
@@ -11458,7 +11533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="386" spans="11:15">
+    <row r="386" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K386" s="1">
         <v>1172</v>
       </c>
@@ -11475,7 +11550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="387" spans="11:15">
+    <row r="387" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K387" s="1">
         <v>1181</v>
       </c>
@@ -11492,7 +11567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="388" spans="11:15">
+    <row r="388" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K388" s="1">
         <v>1184</v>
       </c>
@@ -11509,7 +11584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="389" spans="11:15">
+    <row r="389" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K389" s="1">
         <v>1185</v>
       </c>
@@ -11526,7 +11601,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="390" spans="11:15">
+    <row r="390" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K390" s="1">
         <v>1191</v>
       </c>
@@ -11543,7 +11618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="391" spans="11:15">
+    <row r="391" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K391" s="1">
         <v>1201</v>
       </c>
@@ -11560,7 +11635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="392" spans="11:15">
+    <row r="392" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K392" s="1">
         <v>1203</v>
       </c>
@@ -11577,7 +11652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="393" spans="11:15">
+    <row r="393" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K393" s="1">
         <v>1205</v>
       </c>
@@ -11594,7 +11669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="394" spans="11:15">
+    <row r="394" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K394" s="1">
         <v>1206</v>
       </c>
@@ -11611,7 +11686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="395" spans="11:15">
+    <row r="395" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K395" s="1">
         <v>1209</v>
       </c>
@@ -11628,7 +11703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="396" spans="11:15">
+    <row r="396" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K396" s="1">
         <v>1215</v>
       </c>
@@ -11645,7 +11720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="397" spans="11:15">
+    <row r="397" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K397" s="1">
         <v>1216</v>
       </c>
@@ -11662,7 +11737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="398" spans="11:15">
+    <row r="398" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K398" s="1">
         <v>1220</v>
       </c>
@@ -11679,7 +11754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="399" spans="11:15">
+    <row r="399" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K399" s="1">
         <v>1222</v>
       </c>
@@ -11696,7 +11771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="400" spans="11:15">
+    <row r="400" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K400" s="1">
         <v>1230</v>
       </c>
@@ -11713,7 +11788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="401" spans="11:15">
+    <row r="401" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K401" s="1">
         <v>1231</v>
       </c>
@@ -11730,7 +11805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="402" spans="11:15">
+    <row r="402" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K402" s="1">
         <v>1235</v>
       </c>
@@ -11747,7 +11822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="403" spans="11:15">
+    <row r="403" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K403" s="1">
         <v>1239</v>
       </c>
@@ -11764,7 +11839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="404" spans="11:15">
+    <row r="404" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K404" s="1">
         <v>1241</v>
       </c>
@@ -11781,7 +11856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="405" spans="11:15">
+    <row r="405" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K405" s="1">
         <v>1245</v>
       </c>
@@ -11798,7 +11873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="406" spans="11:15">
+    <row r="406" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K406" s="1">
         <v>1256</v>
       </c>
@@ -11815,7 +11890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="407" spans="11:15">
+    <row r="407" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K407" s="1">
         <v>1266</v>
       </c>
@@ -11832,7 +11907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="408" spans="11:15">
+    <row r="408" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K408" s="1">
         <v>1268</v>
       </c>
@@ -11849,7 +11924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="409" spans="11:15">
+    <row r="409" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K409" s="1">
         <v>1274</v>
       </c>
@@ -11866,7 +11941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="410" spans="11:15">
+    <row r="410" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K410" s="1">
         <v>1275</v>
       </c>
@@ -11883,7 +11958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="411" spans="11:15">
+    <row r="411" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K411" s="1">
         <v>1277</v>
       </c>
@@ -11900,7 +11975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="412" spans="11:15">
+    <row r="412" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K412" s="1">
         <v>1285</v>
       </c>
@@ -11917,7 +11992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="413" spans="11:15">
+    <row r="413" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K413" s="1">
         <v>1289</v>
       </c>
@@ -11934,7 +12009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="414" spans="11:15">
+    <row r="414" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K414" s="1">
         <v>1291</v>
       </c>
@@ -11951,7 +12026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="415" spans="11:15">
+    <row r="415" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K415" s="1">
         <v>1302</v>
       </c>
@@ -11968,7 +12043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="416" spans="11:15">
+    <row r="416" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K416" s="1">
         <v>1358</v>
       </c>
@@ -11985,7 +12060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="417" spans="11:15">
+    <row r="417" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K417" s="1">
         <v>1361</v>
       </c>
@@ -12002,7 +12077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="418" spans="11:15">
+    <row r="418" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K418" s="1">
         <v>1364</v>
       </c>
@@ -12019,7 +12094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="419" spans="11:15">
+    <row r="419" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K419" s="1">
         <v>1369</v>
       </c>
@@ -12036,7 +12111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="420" spans="11:15">
+    <row r="420" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K420" s="1">
         <v>1377</v>
       </c>
@@ -12053,7 +12128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="421" spans="11:15">
+    <row r="421" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K421" s="1">
         <v>1390</v>
       </c>
@@ -12070,7 +12145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="422" spans="11:15">
+    <row r="422" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K422" s="1">
         <v>1397</v>
       </c>
@@ -12087,7 +12162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="423" spans="11:15">
+    <row r="423" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K423" s="1">
         <v>1404</v>
       </c>
@@ -12104,7 +12179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="424" spans="11:15">
+    <row r="424" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K424" s="1">
         <v>1420</v>
       </c>
@@ -12121,7 +12196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="425" spans="11:15">
+    <row r="425" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K425" s="1">
         <v>1427</v>
       </c>
@@ -12138,7 +12213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="426" spans="11:15">
+    <row r="426" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K426" s="1">
         <v>1446</v>
       </c>
@@ -12155,7 +12230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="427" spans="11:15">
+    <row r="427" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K427" s="1">
         <v>1466</v>
       </c>
@@ -12172,7 +12247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="428" spans="11:15">
+    <row r="428" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K428" s="1">
         <v>1470</v>
       </c>
@@ -12189,7 +12264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="429" spans="11:15">
+    <row r="429" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K429" s="1">
         <v>1473</v>
       </c>
@@ -12206,7 +12281,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="430" spans="11:15">
+    <row r="430" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K430" s="1">
         <v>1483</v>
       </c>
@@ -12223,7 +12298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="431" spans="11:15">
+    <row r="431" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K431" s="1">
         <v>1499</v>
       </c>
@@ -12240,7 +12315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="432" spans="11:15">
+    <row r="432" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K432" s="1">
         <v>1510</v>
       </c>
@@ -12257,7 +12332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="433" spans="11:15">
+    <row r="433" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K433" s="1">
         <v>1521</v>
       </c>
@@ -12274,7 +12349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="434" spans="11:15">
+    <row r="434" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K434" s="1">
         <v>1539</v>
       </c>
@@ -12291,7 +12366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="435" spans="11:15">
+    <row r="435" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K435" s="1">
         <v>1576</v>
       </c>
@@ -12308,7 +12383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="436" spans="11:15">
+    <row r="436" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K436" s="1">
         <v>1585</v>
       </c>
@@ -12325,7 +12400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="437" spans="11:15">
+    <row r="437" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K437" s="1">
         <v>1619</v>
       </c>
@@ -12342,7 +12417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="438" spans="11:15">
+    <row r="438" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K438" s="1">
         <v>1643</v>
       </c>
@@ -12359,7 +12434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="439" spans="11:15">
+    <row r="439" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K439" s="1">
         <v>1661</v>
       </c>
@@ -12376,7 +12451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="440" spans="11:15">
+    <row r="440" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K440" s="1">
         <v>1664</v>
       </c>
@@ -12393,7 +12468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="441" spans="11:15">
+    <row r="441" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K441" s="1">
         <v>1672</v>
       </c>
@@ -12410,7 +12485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="442" spans="11:15">
+    <row r="442" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K442" s="1">
         <v>1694</v>
       </c>
@@ -12427,7 +12502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="443" spans="11:15">
+    <row r="443" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K443" s="1">
         <v>1744</v>
       </c>
@@ -12444,7 +12519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="444" spans="11:15">
+    <row r="444" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K444" s="1">
         <v>1765</v>
       </c>
@@ -12461,7 +12536,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="445" spans="11:15">
+    <row r="445" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K445" s="1">
         <v>1824</v>
       </c>
@@ -12478,7 +12553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="446" spans="11:15">
+    <row r="446" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K446" s="1">
         <v>1843</v>
       </c>
@@ -12495,7 +12570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="447" spans="11:15">
+    <row r="447" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K447" s="1">
         <v>1853</v>
       </c>
@@ -12512,7 +12587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="448" spans="11:15">
+    <row r="448" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K448" s="1">
         <v>1901</v>
       </c>
@@ -12529,7 +12604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="449" spans="11:15">
+    <row r="449" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K449" s="1">
         <v>1909</v>
       </c>
@@ -12546,7 +12621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="450" spans="11:15">
+    <row r="450" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K450" s="1">
         <v>1941</v>
       </c>
@@ -12563,7 +12638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="451" spans="11:15">
+    <row r="451" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K451" s="1">
         <v>1992</v>
       </c>
@@ -12580,7 +12655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="452" spans="11:15">
+    <row r="452" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K452" s="1">
         <v>2024</v>
       </c>
@@ -12597,7 +12672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="453" spans="11:15">
+    <row r="453" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K453" s="1">
         <v>2085</v>
       </c>
@@ -12614,7 +12689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="454" spans="11:15">
+    <row r="454" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K454" s="1">
         <v>2150</v>
       </c>
@@ -12631,7 +12706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="455" spans="11:15">
+    <row r="455" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K455" s="1">
         <v>2209</v>
       </c>
@@ -12648,7 +12723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="456" spans="11:15">
+    <row r="456" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K456" s="1">
         <v>2239</v>
       </c>
@@ -12665,7 +12740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="457" spans="11:15">
+    <row r="457" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K457" s="1">
         <v>2302</v>
       </c>
@@ -12682,7 +12757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="458" spans="11:15">
+    <row r="458" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K458" s="1">
         <v>2421</v>
       </c>
@@ -12699,7 +12774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="459" spans="11:15">
+    <row r="459" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K459" s="1">
         <v>2447</v>
       </c>
@@ -12716,7 +12791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="460" spans="11:15">
+    <row r="460" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K460" s="1">
         <v>2758</v>
       </c>
@@ -12733,7 +12808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="461" spans="11:15">
+    <row r="461" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K461" s="1">
         <v>2820</v>
       </c>
@@ -12750,7 +12825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="462" spans="11:15">
+    <row r="462" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K462" s="1">
         <v>3089</v>
       </c>
@@ -12767,7 +12842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="463" spans="11:15">
+    <row r="463" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K463" s="1">
         <v>3145</v>
       </c>
@@ -12784,7 +12859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="464" spans="11:15">
+    <row r="464" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K464" s="1">
         <v>3167</v>
       </c>
@@ -12801,7 +12876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="465" spans="11:15">
+    <row r="465" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K465" s="1">
         <v>3341</v>
       </c>
@@ -12818,7 +12893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="466" spans="11:15">
+    <row r="466" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K466" s="1">
         <v>4063</v>
       </c>

</xml_diff>